<commit_message>
#32072 updated requirements document and approval added
</commit_message>
<xml_diff>
--- a/Documents/External/Requirements CommLib CML000001 v0.1 Document Review Sheet.xlsx
+++ b/Documents/External/Requirements CommLib CML000001 v0.1 Document Review Sheet.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27715"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/310035243p/Documents/OneDrive - Philips/DI/Horizontal/CommLib/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/310088528p/dev/android-commlib-workspace/Source/commlib/Documents/External/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="904" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" tabRatio="904" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Title Page" sheetId="3" r:id="rId1"/>
     <sheet name="Logging" sheetId="19" r:id="rId2"/>
-    <sheet name="&lt;Use Instruction - Delete&gt;" sheetId="16" r:id="rId3"/>
   </sheets>
   <externalReferences>
+    <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
-    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="col">#REF!</definedName>
@@ -43,24 +42,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Purpose</t>
   </si>
   <si>
     <t>Scope</t>
-  </si>
-  <si>
-    <t>&lt;Fill in Instruction. Remove this tab when completing the document&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;When printing the document make sure all pages all legable with right page numbering and document identification.
-Ensure the printed version has correct:
-- Orientation
-- Print Area
-- Page Breaks
-- Scaling 
-</t>
   </si>
   <si>
     <t>This Document Review Sheet template is used during formal document reviews to capture the reviewer's feedback.</t>
@@ -93,34 +80,21 @@
     <t>Verified? (Y/N)</t>
   </si>
   <si>
-    <t>Fill-in instructions for the user of the Document review sheet template
-Update the header and footer properties of all Excel sheets:
-• Select all sheets (Select first sheets, press shift ket, use right mouse button to select all sheets)
-• Update footer doc Id, version and status
-• Replace the &lt;Subject&gt; in the header by the actual subject 
-          • Example: Document Review Sheet CDPP-P-02000002 QMS Document and record control procedure
-Update Title Sheet:
-Update the table part with the document properties with:
-• Fill in the review sheet doc id at Doc ID (as used in local document management system)
-• Update the author field with the authors name of the deliverable
-All chapters and tables in this document that require information to be entered must be completed.
-For content not applicable fill in “Not Applicable” or ‘NA’ and include justification.
-Fill out the template in line with the instruction to create the deliverable and delete all red explanatory text before finalizing the document.
-When adding new tabs  use same footer layout as in the Title tab. Page layout &gt; Print Titles &gt; Header/Footer &gt; Custom Footer&gt;</t>
-  </si>
-  <si>
     <t>CML000001 Requirements CommLib 0.1</t>
   </si>
   <si>
     <t>Document: CML000001 Requirements CommLib 0.1
 Product/Platform: CDP²</t>
   </si>
+  <si>
+    <t>no review comments (Bas Flaton)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,42 +132,9 @@
       <family val="2"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="5"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="14"/>
-      <color theme="5"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FFC0504D"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -291,36 +232,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -341,19 +267,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -362,13 +288,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -409,16 +335,16 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1066,148 +992,148 @@
     <col min="2" max="2" width="22.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="11.83203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="23.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="5.5" style="10" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="5.5" style="5" customWidth="1"/>
     <col min="7" max="7" width="16" style="2" customWidth="1"/>
     <col min="8" max="8" width="22.5" style="2" customWidth="1"/>
     <col min="9" max="16384" width="20" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
-        <v>4</v>
+      <c r="A2" s="34" t="s">
+        <v>2</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
     </row>
     <row r="5" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="42" t="s">
-        <v>15</v>
+      <c r="A5" s="36" t="s">
+        <v>12</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
     </row>
     <row r="6" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="39" t="s">
-        <v>16</v>
+      <c r="A6" s="34" t="s">
+        <v>13</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G15" s="10"/>
+      <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G16" s="10"/>
+      <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G17" s="10"/>
+      <c r="G17" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="10"/>
+      <c r="A20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
@@ -1218,7 +1144,7 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A5:H5"/>
   </mergeCells>
-  <phoneticPr fontId="14" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="1.2480314960000001" header="0.31496062992126" footer="0.31496063000000002"/>
   <pageSetup paperSize="9" scale="92" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
@@ -1238,7 +1164,7 @@
   <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1251,524 +1177,526 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="B4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="16"/>
-    </row>
-    <row r="4" spans="1:9" customFormat="1" ht="26" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+      <c r="C4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="D4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="E4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="F4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="G4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="21" t="s">
-        <v>12</v>
+    </row>
+    <row r="5" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="19"/>
+      <c r="I5" s="21"/>
+    </row>
+    <row r="6" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="22" t="s">
+        <v>14</v>
       </c>
-      <c r="G4" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="24"/>
-      <c r="I5" s="26"/>
-    </row>
-    <row r="6" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="30"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="25"/>
     </row>
     <row r="7" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="30"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="8" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="30"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="25"/>
     </row>
     <row r="9" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="30"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="25"/>
     </row>
     <row r="10" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="30"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="25"/>
     </row>
     <row r="11" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="30"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="25"/>
     </row>
     <row r="12" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="30"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="25"/>
     </row>
     <row r="13" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="30"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="25"/>
     </row>
     <row r="14" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="30"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="25"/>
     </row>
     <row r="15" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="30"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="25"/>
     </row>
     <row r="16" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="30"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="25"/>
     </row>
     <row r="17" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="30"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="25"/>
     </row>
     <row r="18" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="30"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="25"/>
     </row>
     <row r="19" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="30"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="25"/>
     </row>
     <row r="20" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="30"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="25"/>
     </row>
     <row r="21" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="30"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="25"/>
     </row>
     <row r="22" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="30"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="25"/>
     </row>
     <row r="23" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="30"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="25"/>
     </row>
     <row r="24" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="30"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="25"/>
     </row>
     <row r="25" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="30"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="25"/>
     </row>
     <row r="26" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="22"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="30"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="25"/>
     </row>
     <row r="27" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="30"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="25"/>
     </row>
     <row r="28" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="30"/>
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="25"/>
     </row>
     <row r="29" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="34"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="30"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="25"/>
     </row>
     <row r="30" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="22"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="30"/>
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="25"/>
     </row>
     <row r="31" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="22"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="30"/>
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="25"/>
     </row>
     <row r="32" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="22"/>
-      <c r="B32" s="35"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="30"/>
+      <c r="A32" s="17"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="25"/>
     </row>
     <row r="33" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" s="22"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="30"/>
+      <c r="A33" s="17"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="25"/>
     </row>
     <row r="34" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" s="22"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="30"/>
+      <c r="A34" s="17"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="25"/>
     </row>
     <row r="35" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="34"/>
-      <c r="B35" s="22"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="30"/>
+      <c r="A35" s="29"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="25"/>
     </row>
     <row r="36" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="22"/>
-      <c r="B36" s="22"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="28"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="30"/>
+      <c r="A36" s="17"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="25"/>
     </row>
     <row r="37" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="22"/>
-      <c r="B37" s="22"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="28"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="30"/>
+      <c r="A37" s="17"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="25"/>
     </row>
     <row r="38" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A38" s="22"/>
-      <c r="B38" s="22"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="28"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="30"/>
+      <c r="A38" s="17"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="25"/>
     </row>
     <row r="39" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A39" s="34"/>
-      <c r="B39" s="22"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="30"/>
+      <c r="A39" s="29"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="25"/>
     </row>
     <row r="40" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A40" s="34"/>
-      <c r="B40" s="22"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="28"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="30"/>
+      <c r="A40" s="29"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="25"/>
     </row>
     <row r="41" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A41" s="22"/>
-      <c r="B41" s="22"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="28"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="30"/>
+      <c r="A41" s="17"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="25"/>
     </row>
     <row r="42" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A42" s="22"/>
-      <c r="B42" s="22"/>
-      <c r="C42" s="27"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="28"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="30"/>
+      <c r="A42" s="17"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="25"/>
     </row>
     <row r="43" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A43" s="37"/>
-      <c r="B43" s="22"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="30"/>
-      <c r="F43" s="38"/>
-      <c r="G43" s="30"/>
+      <c r="A43" s="32"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="25"/>
     </row>
     <row r="44" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A44" s="37"/>
-      <c r="B44" s="22"/>
-      <c r="C44" s="27"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="30"/>
-      <c r="F44" s="38"/>
-      <c r="G44" s="30"/>
+      <c r="A44" s="32"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="25"/>
     </row>
     <row r="45" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A45" s="37"/>
-      <c r="B45" s="22"/>
-      <c r="C45" s="27"/>
-      <c r="D45" s="23"/>
-      <c r="E45" s="30"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="30"/>
+      <c r="A45" s="32"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="25"/>
     </row>
     <row r="46" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A46" s="37"/>
-      <c r="B46" s="22"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="23"/>
-      <c r="E46" s="30"/>
-      <c r="F46" s="38"/>
-      <c r="G46" s="30"/>
+      <c r="A46" s="32"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="25"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="25"/>
     </row>
     <row r="47" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A47" s="37"/>
-      <c r="B47" s="22"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="23"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="38"/>
-      <c r="G47" s="30"/>
+      <c r="A47" s="32"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A48" s="37"/>
-      <c r="B48" s="22"/>
-      <c r="C48" s="27"/>
-      <c r="D48" s="23"/>
-      <c r="E48" s="30"/>
-      <c r="F48" s="38"/>
-      <c r="G48" s="30"/>
+      <c r="A48" s="32"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="25"/>
     </row>
     <row r="49" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A49" s="37"/>
-      <c r="B49" s="22"/>
-      <c r="C49" s="27"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="38"/>
-      <c r="G49" s="30"/>
+      <c r="A49" s="32"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="33"/>
+      <c r="G49" s="25"/>
     </row>
     <row r="50" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A50" s="37"/>
-      <c r="B50" s="22"/>
-      <c r="C50" s="27"/>
-      <c r="D50" s="23"/>
-      <c r="E50" s="30"/>
-      <c r="F50" s="38"/>
-      <c r="G50" s="30"/>
+      <c r="A50" s="32"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="33"/>
+      <c r="G50" s="25"/>
     </row>
     <row r="51" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A51" s="37"/>
-      <c r="B51" s="22"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="23"/>
-      <c r="E51" s="30"/>
-      <c r="F51" s="38"/>
-      <c r="G51" s="30"/>
+      <c r="A51" s="32"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="25"/>
+      <c r="F51" s="33"/>
+      <c r="G51" s="25"/>
     </row>
     <row r="52" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A52" s="37"/>
-      <c r="B52" s="22"/>
-      <c r="C52" s="27"/>
-      <c r="D52" s="23"/>
-      <c r="E52" s="30"/>
-      <c r="F52" s="38"/>
-      <c r="G52" s="30"/>
+      <c r="A52" s="32"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="22"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="25"/>
+      <c r="F52" s="33"/>
+      <c r="G52" s="25"/>
     </row>
     <row r="53" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A53" s="37"/>
-      <c r="B53" s="22"/>
-      <c r="C53" s="27"/>
-      <c r="D53" s="23"/>
-      <c r="E53" s="30"/>
-      <c r="F53" s="38"/>
-      <c r="G53" s="30"/>
+      <c r="A53" s="32"/>
+      <c r="B53" s="17"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="33"/>
+      <c r="G53" s="25"/>
     </row>
     <row r="54" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A54" s="37"/>
-      <c r="B54" s="22"/>
-      <c r="C54" s="27"/>
-      <c r="D54" s="23"/>
-      <c r="E54" s="30"/>
-      <c r="F54" s="38"/>
-      <c r="G54" s="30"/>
+      <c r="A54" s="32"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="33"/>
+      <c r="G54" s="25"/>
     </row>
     <row r="55" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A55" s="37"/>
-      <c r="B55" s="22"/>
-      <c r="C55" s="27"/>
-      <c r="D55" s="23"/>
-      <c r="E55" s="30"/>
-      <c r="F55" s="38"/>
-      <c r="G55" s="30"/>
+      <c r="A55" s="32"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="33"/>
+      <c r="G55" s="25"/>
     </row>
     <row r="56" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A56" s="37"/>
-      <c r="B56" s="22"/>
-      <c r="C56" s="27"/>
-      <c r="D56" s="23"/>
-      <c r="E56" s="30"/>
-      <c r="F56" s="38"/>
-      <c r="G56" s="30"/>
+      <c r="A56" s="32"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="25"/>
+      <c r="F56" s="33"/>
+      <c r="G56" s="25"/>
     </row>
     <row r="57" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A57" s="37"/>
-      <c r="B57" s="22"/>
-      <c r="C57" s="27"/>
-      <c r="D57" s="23"/>
-      <c r="E57" s="30"/>
-      <c r="F57" s="38"/>
-      <c r="G57" s="30"/>
+      <c r="A57" s="32"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="22"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="25"/>
+      <c r="F57" s="33"/>
+      <c r="G57" s="25"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="14" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <conditionalFormatting sqref="D14 D5:D12">
     <cfRule type="expression" dxfId="29" priority="29" stopIfTrue="1">
       <formula>OR(D5="S",D5="Ma",D5="mi",D5="cl",D5="Q")</formula>
@@ -1899,56 +1827,6 @@
   </dataValidations>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="1.2480314960000001" header="0.31496062992126" footer="0.31496063000000002"/>
   <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Arial,Regular"&amp;20&amp;K000000Document Review Sheet &amp;K05+000&lt;Document ID and Title&gt;</oddHeader>
-    <oddFooter>&amp;L&amp;12Doc ID: &lt;doc ID&gt;
-Version: &lt;N.M&gt;
-Status: &lt; Approved&gt;
-&amp;CDocument Title:   
-&lt;Template Title&gt; &lt; Subject&gt;   
-Template ID: CDPP-T-02000003 Template Version: 1.0
-Printed copies are uncontrolled unless authenticated&amp;RAuthor: &lt;author&gt;
-Approver: &lt;approver&gt;</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0">
-    <tabColor rgb="FFC0504D"/>
-  </sheetPr>
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="130.5" style="8" customWidth="1"/>
-    <col min="2" max="2" width="140" style="8" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="8"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" s="6" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="370.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="105" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="1.2480314960000001" header="0.31496062992126" footer="0.31496063000000002"/>
-  <pageSetup paperSize="9" scale="92" fitToHeight="100" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;20&amp;K000000Document Review Sheet &amp;K05+000&lt;Document ID and Title&gt;</oddHeader>
     <oddFooter>&amp;L&amp;12Doc ID: &lt;doc ID&gt;

</xml_diff>